<commit_message>
Work in progress on Format ID Guide
</commit_message>
<xml_diff>
--- a/db/seed_data/formats.xlsx
+++ b/db/seed_data/formats.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="5700" yWindow="340" windowWidth="20960" windowHeight="14900"/>
   </bookViews>
   <sheets>
-    <sheet name="Optical Media" sheetId="1" r:id="rId1"/>
+    <sheet name="Formats" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -42,9 +42,6 @@
     <t>Synonyms</t>
   </si>
   <si>
-    <t>Digital video disc; Digital versatile disc</t>
-  </si>
-  <si>
     <t>Dates</t>
   </si>
   <si>
@@ -155,16 +152,6 @@
   </si>
   <si>
     <t>Polycarbonate plastic disc substrate coated with a thin, reflective "data layer" composed of metal (commercial CDs) or dyes (recordable, rewritable CDs)</t>
-  </si>
-  <si>
-    <t>Compact discs. Image by Lori Dedeyan, available under a Creative Commons Attribution-NonCommercial-ShareAlike license (&lt;a href="https://creativecommons.org/licenses/by-nc-sa/2.0/" 
-target="_blank"&gt;CC BY-NC-SA 2.0&lt;/a&gt;). Courtesy of UCLA Library Special Collections.; CD-R in jewel case.; Evident CD-R disc rot on top of disc.; Evident CD-R disc rot on bottom of disc.</t>
-  </si>
-  <si>
-    <t>cds-ucla.jpg; compactdisc-gold-jewelcase.jpg; cd-rot-spotting.jpg; cd-rot-spotting1b.jpg</t>
-  </si>
-  <si>
-    <t>Three compact discs; CD-R in jewel case; Evident spots of CD-R disc rot - top view; Evident spots of CD-R disc rot - bottom view</t>
   </si>
   <si>
     <t>Most CD damage is incurred through poor storage and handling. Surface scratches, gouges, and smudges can inhibit playback of the disc. There may be some inherent vice within the materials used to create CDs, but signal loss due to inherent vice is not as frequent in newer CDs. If the seal encasing the aluminum recording surface is somehow compromised, the aluminum layer can oxidize, resulting in data loss. This deterioration is colloquially referred to as "disc rot" or "laser rot." Indications of disc rot include: pin-sized holes in the reflective layer, a bronze coloring on the non-labeled side of the disc, and crazing. Crazing can be seen in snowflake-like or fractal-like milky-white patterns on the disc. Crazing typically only affects early CDs because as manufacturing processes improved, the issue became less of a problem. Scratches on the label side of CDs can also affect playback, since CDs are relatively thin and composed of a single layer of reflective aluminum encased in polycarbonate. Any discs that exhibit these signs of deterioration should be error checked and/or replaced.
@@ -207,16 +194,6 @@
     <t>Acrylic disc containing a thin, reflective aluminum "data layer"; various types of adhesive were used to sandwich the two acrylic disc sides</t>
   </si>
   <si>
-    <t>laserdisc-scale-ucla.jpg; laserdisc-surface.jpg; laserdisc-rot01.jpg</t>
-  </si>
-  <si>
-    <t>Laserdisc in sleeve; Laserdisc surface; LaserDisc rot</t>
-  </si>
-  <si>
-    <t>Laserdisc. Image by Lori Dedeyan, available under a Creative Commons Attribution-NonCommercial-ShareAlike license (&lt;a href="https://creativecommons.org/licenses/by-nc-sa/2.0/" 
-target="_blank"&gt;CC BY-NC-SA 2.0&lt;/a&gt;). Courtesy of UCLA Library Special Collections.; Iridescent Laserdisc surface. Image by Wikimedia Commons user Autopilot, available under a Creative Commons Attribution-ShareAlike license (&lt;a href="http://creativecommons.org/licenses/by-sa/3.0/deed.en" target="_blank"&gt;CC BY-SA 3.0&lt;/a&gt;); Laserdisc (manufactured 1983) exhibiting "laser rot" damage. Image by Wikimedia Commons user Marcus Rowland, available under a Creative Commons Attribution-ShareAlike license (&lt;a href="http://creativecommons.org/licenses/by-sa/3.0/deed.en" target="_blank"&gt;CC BY-SA 3.0&lt;/a&gt;)</t>
-  </si>
-  <si>
     <t>LaserDiscs are subject to mechanical and surface contaminants. Scratches and dirt can drastically affect laser performance, as playback equipment can become misaligned and mistracked. Additionally, LaserDiscs do not have some of the error correction technology that later optical media have, and they are much more sensitive to damage.
 Inherent vice also affects LaserDisc. Some manufacturing defects adversely affect the lifespan and playback quality of the discs. Discs may succumb to surface crazing, where the surface of the discs exhibits a milky white, lattice, or spider web-like pattern. Crazing can indicate that the seal which protects the inner aluminum signal carrier has broken, making the inner core vulnerable to oxidation. Oxidation is also known as laser rot, as the aluminum loses its reflectivity and the quality of the playback signal degrades. Oxidation of the delicate aluminum can render the signal irretrievable.</t>
   </si>
@@ -246,15 +223,6 @@
       &lt;/tr&gt;
     &lt;/tbody&gt;
     &lt;/table&gt;</t>
-  </si>
-  <si>
-    <t>minidisc-sony-frontandback.jpg; minidisc-memorex.jpg</t>
-  </si>
-  <si>
-    <t>Minidisc front and back views; Memorex MiniDisc</t>
-  </si>
-  <si>
-    <t>&gt;MiniDisc cartridge: front and back views.; MiniDisc cartridge. Image by Wikimedia Commons user Evan-Amos, image available under the public domain.</t>
   </si>
   <si>
     <t>c. 1992 &amp;ndash; c. 2013;  use persists, manufacturing ended in 2013</t>
@@ -381,6 +349,42 @@
   </si>
   <si>
     <t>Anchor</t>
+  </si>
+  <si>
+    <t>cds-ucla.jpg||compactdisc-gold-jewelcase.jpg||cd-rot-spotting.jpg||cd-rot-spotting1b.jpg</t>
+  </si>
+  <si>
+    <t>laserdisc-scale-ucla.jpg||laserdisc-surface.jpg||laserdisc-rot01.jpg</t>
+  </si>
+  <si>
+    <t>minidisc-sony-frontandback.jpg||minidisc-memorex.jpg</t>
+  </si>
+  <si>
+    <t>MiniDisc cartridge: front and back views.||MiniDisc cartridge. Image by Wikimedia Commons user Evan-Amos, image available under the public domain.</t>
+  </si>
+  <si>
+    <t>Laserdisc. Image by Lori Dedeyan, available under a Creative Commons Attribution-NonCommercial-ShareAlike license (&lt;a href="https://creativecommons.org/licenses/by-nc-sa/2.0/" 
+target="_blank"&gt;CC BY-NC-SA 2.0&lt;/a&gt;). Courtesy of UCLA Library Special Collections.||Iridescent Laserdisc surface. Image by Wikimedia Commons user Autopilot, available under a Creative Commons Attribution-ShareAlike license (&lt;a href="http://creativecommons.org/licenses/by-sa/3.0/deed.en" target="_blank"&gt;CC BY-SA 3.0&lt;/a&gt;); Laserdisc (manufactured 1983) exhibiting "laser rot" damage. Image by Wikimedia Commons user Marcus Rowland, available under a Creative Commons Attribution-ShareAlike license (&lt;a href="http://creativecommons.org/licenses/by-sa/3.0/deed.en" target="_blank"&gt;CC BY-SA 3.0&lt;/a&gt;)</t>
+  </si>
+  <si>
+    <t>Compact discs. Image by Lori Dedeyan, available under a Creative Commons Attribution-NonCommercial-ShareAlike license (&lt;a href="https://creativecommons.org/licenses/by-nc-sa/2.0/" 
+target="_blank"&gt;CC BY-NC-SA 2.0&lt;/a&gt;). Courtesy of UCLA Library Special Collections.||CD-R in jewel case.||Evident CD-R disc rot on top of disc.||Evident CD-R disc rot on bottom of disc.</t>
+  </si>
+  <si>
+    <t>Three compact discs||CD-R in jewel case||Evident spots of CD-R disc rot - top view||Evident spots of CD-R disc rot - bottom view</t>
+  </si>
+  <si>
+    <t>Laserdisc in sleeve||Laserdisc surface||LaserDisc rot</t>
+  </si>
+  <si>
+    <t>Minidisc front and back views||Memorex MiniDisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+    &lt;li&gt;Digital video disc&lt;/li&gt;
+    &lt;li&gt;Digital versatile disc&lt;/li&gt;
+&lt;/ul&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -429,8 +433,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -441,9 +451,15 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -714,7 +730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -727,7 +743,7 @@
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -757,312 +773,312 @@
   <sheetData>
     <row r="1" spans="1:21" ht="30.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>78</v>
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="R4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="S5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>